<commit_message>
error : 'Object of type 'int64' is not JSON serializable' is asolved
</commit_message>
<xml_diff>
--- a/dummy-data-product/src/output/data_info.xlsx
+++ b/dummy-data-product/src/output/data_info.xlsx
@@ -489,13 +489,13 @@
         <v>-15</v>
       </c>
       <c r="I2">
-        <v>15</v>
+        <v>35.45</v>
       </c>
       <c r="J2">
         <v>12907.5</v>
       </c>
       <c r="K2">
-        <v>14407.5</v>
+        <v>15430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>